<commit_message>
Prepared for Spira execution
</commit_message>
<xml_diff>
--- a/Data100.xlsx
+++ b/Data100.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22430"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\Inflectra\InflectraGitProjects\rapise-demo\DynamicsNAV\NavFramework\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F64D3C85-BBB2-49BD-AB69-D7CA13F53F45}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1000" yWindow="1000" windowWidth="15000" windowHeight="10000" activeTab="1"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="14060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CreateNewCustomer" sheetId="1" r:id="rId1"/>
@@ -23,9 +29,6 @@
     <t>Elkhorn Airport</t>
   </si>
   <si>
-    <t>y</t>
-  </si>
-  <si>
     <t>Country</t>
   </si>
   <si>
@@ -114,26 +117,29 @@
   </si>
   <si>
     <t>TAXABLE</t>
+  </si>
+  <si>
+    <t>n</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <color theme="1"/>
-      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <b/>
-      <color theme="1"/>
-      <sz val="11"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -146,7 +152,7 @@
     </fill>
   </fills>
   <borders count="1">
-    <border outline="0">
+    <border>
       <left/>
       <right/>
       <top/>
@@ -168,6 +174,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -455,187 +469,175 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
-    <pageSetUpPr/>
   </sheetPr>
   <dimension ref="A1:H2"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" zoomScaleSheetLayoutView="60" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection activeCell="$A$2" sqref="$A$2:$A$2"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="24.42578125" customWidth="1"/>
+    <col min="1" max="1" width="24.453125" customWidth="1"/>
     <col min="2" max="2" width="14.1796875" customWidth="1"/>
     <col min="3" max="3" width="21.26953125" customWidth="1"/>
-    <col min="4" max="5" width="8.7265625"/>
     <col min="6" max="6" width="11.1796875" customWidth="1"/>
     <col min="7" max="7" width="33.26953125" customWidth="1"/>
-    <col min="8" max="8" width="18.359375" customWidth="1"/>
-    <col min="9" max="16384" width="8.7265625"/>
+    <col min="8" max="8" width="18.36328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>20</v>
-      </c>
       <c r="G1" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="H1" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C2" t="s">
-        <v>30</v>
-      </c>
       <c r="D2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E2">
         <v>20910</v>
       </c>
       <c r="F2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H2" t="s">
-        <v>1</v>
+        <v>31</v>
       </c>
     </row>
   </sheetData>
-  <sheetProtection/>
-  <printOptions/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
-    <pageSetUpPr/>
   </sheetPr>
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="60" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection activeCell="$C$3" sqref="$C$3:$C$3"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="24.42578125" customWidth="1"/>
+    <col min="1" max="1" width="24.453125" customWidth="1"/>
     <col min="2" max="2" width="13.90625" customWidth="1"/>
     <col min="3" max="3" width="12.08984375" style="2" customWidth="1"/>
-    <col min="4" max="16384" width="8.7265625"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
         <v>9</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="s">
-        <v>10</v>
       </c>
       <c r="B2" t="s">
         <v>0</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>
-  <sheetProtection/>
-  <printOptions/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
-    <pageSetUpPr/>
   </sheetPr>
   <dimension ref="A1:G3"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" zoomScaleSheetLayoutView="60" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection activeCell="$A$1" sqref="$A$1:$C$3"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection sqref="A1:C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="11.36328125" customWidth="1"/>
-    <col min="2" max="2" width="8.7265625"/>
     <col min="3" max="3" width="14.54296875" customWidth="1"/>
     <col min="4" max="4" width="13.36328125" customWidth="1"/>
     <col min="5" max="5" width="11.7265625" customWidth="1"/>
     <col min="6" max="6" width="9.36328125" customWidth="1"/>
     <col min="7" max="7" width="11.81640625" customWidth="1"/>
-    <col min="8" max="16384" width="8.7265625"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="F1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="2">
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -644,7 +646,7 @@
         <v>4000</v>
       </c>
       <c r="D2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E2">
         <v>5</v>
@@ -656,9 +658,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B3">
         <v>2</v>
@@ -667,7 +669,7 @@
         <v>1000</v>
       </c>
       <c r="D3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E3">
         <v>10</v>
@@ -680,93 +682,85 @@
       </c>
     </row>
   </sheetData>
-  <sheetProtection/>
-  <printOptions/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
-    <pageSetUpPr/>
   </sheetPr>
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" zoomScaleSheetLayoutView="60" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection activeCell="$A$2" sqref="$A$2:$A$2"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="24.42578125" customWidth="1"/>
-    <col min="2" max="16384" width="8.7265625"/>
+    <col min="1" max="1" width="24.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>27</v>
-      </c>
       <c r="C1" s="3" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="2">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
   </sheetData>
-  <sheetProtection/>
-  <printOptions/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
-    <pageSetUpPr/>
   </sheetPr>
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" zoomScaleSheetLayoutView="60" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection activeCell="$C$4" sqref="$C$4:$C$4"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="11.36328125" customWidth="1"/>
     <col min="2" max="2" width="8.36328125" customWidth="1"/>
     <col min="3" max="3" width="14.6328125" customWidth="1"/>
-    <col min="4" max="16384" width="8.7265625"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="2">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B2">
         <v>5</v>
@@ -775,9 +769,9 @@
         <v>350</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B3">
         <v>10</v>
@@ -787,8 +781,6 @@
       </c>
     </row>
   </sheetData>
-  <sheetProtection/>
-  <printOptions/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>